<commit_message>
Updated the IAQ beacon part list
</commit_message>
<xml_diff>
--- a/Important_Documents/BeaconIAQ_PartList.xlsx
+++ b/Important_Documents/BeaconIAQ_PartList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagenfritz/Google Drive/Research/IEL/Projects/bevo_iaq/Important Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagenfritz/Google Drive/Research/IEL/Projects/bevo_iaq/Important_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DA058C-3349-DB49-BF22-FC4D7A7161B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F03E68-DFC4-D345-A0C4-F748A193A2E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{7BD9F167-FFFC-1744-BC8E-DFE7BF7352B7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="149">
   <si>
     <t>Part</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Shipping - PCBway.com</t>
   </si>
   <si>
-    <t>Shipping - Pololu</t>
-  </si>
-  <si>
     <t>https://www.pololu.com/cart?submit=view_cart#shipping-estimate</t>
   </si>
   <si>
@@ -472,6 +469,15 @@
   </si>
   <si>
     <t>Price per Beacon</t>
+  </si>
+  <si>
+    <t>Shipping - Amazon.com</t>
+  </si>
+  <si>
+    <t>Shipping - Pololu.com</t>
+  </si>
+  <si>
+    <t>www.amazon.com</t>
   </si>
 </sst>
 </file>
@@ -967,15 +973,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="4" borderId="15" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -996,6 +993,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1312,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8126A4BC-CD52-C544-BC25-D87F7F426AEE}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1331,23 +1337,23 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="51"/>
-      <c r="H2" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="53" t="s">
+      <c r="D2" s="71"/>
+      <c r="H2" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="51" t="s">
         <v>97</v>
-      </c>
-      <c r="J2" s="54" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1355,16 +1361,16 @@
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" s="63" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1372,16 +1378,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" s="57" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="H4" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1389,16 +1395,16 @@
         <v>12</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="J5" s="57" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="H5" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1406,16 +1412,16 @@
         <v>13</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="I6" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" s="57" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="H6" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="54" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1423,16 +1429,16 @@
         <v>14</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="I7" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="57" t="s">
         <v>89</v>
-      </c>
-      <c r="J7" s="60" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1440,8 +1446,8 @@
       <c r="A9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="64" t="s">
-        <v>120</v>
+      <c r="B9" s="61" t="s">
+        <v>119</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>2</v>
@@ -1450,27 +1456,27 @@
         <v>1</v>
       </c>
       <c r="E9" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="33" t="s">
         <v>145</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>146</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="H9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" t="s">
         <v>108</v>
-      </c>
-      <c r="I9" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="65" t="s">
-        <v>110</v>
+      <c r="B10" s="62" t="s">
+        <v>109</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>3</v>
@@ -1482,25 +1488,25 @@
         <v>46.71</v>
       </c>
       <c r="F10" s="35">
-        <f>D10*E10</f>
+        <f t="shared" ref="F10:F22" si="0">D10*E10</f>
         <v>46.71</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
-        <v>111</v>
+      <c r="B11" s="63" t="s">
+        <v>110</v>
       </c>
       <c r="C11" s="36" t="s">
         <v>3</v>
@@ -1512,25 +1518,25 @@
         <v>24.26</v>
       </c>
       <c r="F11" s="37">
-        <f>D11*E11</f>
+        <f t="shared" si="0"/>
         <v>24.26</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="66" t="s">
-        <v>112</v>
+      <c r="B12" s="63" t="s">
+        <v>111</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>3</v>
@@ -1542,25 +1548,25 @@
         <v>57.5</v>
       </c>
       <c r="F12" s="37">
-        <f>D12*E12</f>
+        <f t="shared" si="0"/>
         <v>57.5</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="66" t="s">
-        <v>113</v>
+      <c r="B13" s="63" t="s">
+        <v>112</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>3</v>
@@ -1572,25 +1578,25 @@
         <v>6.95</v>
       </c>
       <c r="F13" s="37">
-        <f>D13*E13</f>
+        <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="66" t="s">
-        <v>114</v>
+      <c r="B14" s="63" t="s">
+        <v>113</v>
       </c>
       <c r="C14" s="36" t="s">
         <v>3</v>
@@ -1602,25 +1608,25 @@
         <v>75</v>
       </c>
       <c r="F14" s="37">
-        <f>D14*E14</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="66" t="s">
-        <v>115</v>
+      <c r="B15" s="63" t="s">
+        <v>114</v>
       </c>
       <c r="C15" s="36" t="s">
         <v>3</v>
@@ -1632,25 +1638,25 @@
         <v>75</v>
       </c>
       <c r="F15" s="37">
-        <f>D15*E15</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="67" t="s">
-        <v>116</v>
+      <c r="B16" s="64" t="s">
+        <v>115</v>
       </c>
       <c r="C16" s="38" t="s">
         <v>9</v>
@@ -1663,25 +1669,25 @@
         <v>2.7450000000000001</v>
       </c>
       <c r="F16" s="39">
-        <f>D16*E16</f>
+        <f t="shared" si="0"/>
         <v>2.7450000000000001</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="67" t="s">
-        <v>117</v>
+      <c r="B17" s="64" t="s">
+        <v>116</v>
       </c>
       <c r="C17" s="38" t="s">
         <v>9</v>
@@ -1693,25 +1699,25 @@
         <v>40</v>
       </c>
       <c r="F17" s="39">
-        <f>D17*E17</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="67" t="s">
-        <v>118</v>
+        <v>99</v>
+      </c>
+      <c r="B18" s="64" t="s">
+        <v>117</v>
       </c>
       <c r="C18" s="38" t="s">
         <v>9</v>
@@ -1723,25 +1729,25 @@
         <v>9.99</v>
       </c>
       <c r="F18" s="39">
-        <f>D18*E18</f>
+        <f t="shared" si="0"/>
         <v>9.99</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="68" t="s">
-        <v>119</v>
+      <c r="B19" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="C19" s="40" t="s">
         <v>14</v>
@@ -1754,25 +1760,25 @@
         <v>6.759729272419629E-2</v>
       </c>
       <c r="F19" s="41">
-        <f>D19*E19</f>
+        <f t="shared" si="0"/>
         <v>6.759729272419629E-2</v>
       </c>
       <c r="G19" s="23" t="s">
         <v>25</v>
       </c>
       <c r="H19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="69" t="s">
-        <v>121</v>
+      <c r="B20" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>13</v>
@@ -1785,25 +1791,25 @@
         <v>0.19980000000000001</v>
       </c>
       <c r="F20" s="43">
-        <f>D20*E20</f>
+        <f t="shared" si="0"/>
         <v>0.79920000000000002</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="69" t="s">
-        <v>121</v>
+      <c r="B21" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="C21" s="42" t="s">
         <v>13</v>
@@ -1816,25 +1822,25 @@
         <v>0.29799999999999999</v>
       </c>
       <c r="F21" s="43">
-        <f>D21*E21</f>
+        <f t="shared" si="0"/>
         <v>1.1919999999999999</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>30</v>
       </c>
       <c r="H21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="69" t="s">
-        <v>122</v>
+      <c r="B22" s="66" t="s">
+        <v>121</v>
       </c>
       <c r="C22" s="42" t="s">
         <v>13</v>
@@ -1847,25 +1853,25 @@
         <v>0.1158</v>
       </c>
       <c r="F22" s="43">
-        <f>D22*E22</f>
+        <f t="shared" si="0"/>
         <v>0.2316</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="69" t="s">
-        <v>121</v>
+      <c r="B23" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="C23" s="42" t="s">
         <v>13</v>
@@ -1878,25 +1884,25 @@
         <v>9.9833333333333343E-2</v>
       </c>
       <c r="F23" s="43">
-        <f>E23*D23</f>
+        <f t="shared" ref="F23:F51" si="1">E23*D23</f>
         <v>0.39933333333333337</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>34</v>
       </c>
       <c r="H23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="69" t="s">
-        <v>122</v>
+      <c r="B24" s="66" t="s">
+        <v>121</v>
       </c>
       <c r="C24" s="42" t="s">
         <v>13</v>
@@ -1909,25 +1915,25 @@
         <v>7.4874999999999997E-2</v>
       </c>
       <c r="F24" s="43">
-        <f>E24*D24</f>
+        <f t="shared" si="1"/>
         <v>0.14974999999999999</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>36</v>
       </c>
       <c r="H24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="70" t="s">
-        <v>123</v>
+      <c r="B25" s="67" t="s">
+        <v>122</v>
       </c>
       <c r="C25" s="44" t="s">
         <v>12</v>
@@ -1940,25 +1946,25 @@
         <v>2.3599999999999999E-2</v>
       </c>
       <c r="F25" s="45">
-        <f>E25*D25</f>
+        <f t="shared" si="1"/>
         <v>2.3599999999999999E-2</v>
       </c>
       <c r="G25" s="27" t="s">
         <v>43</v>
       </c>
       <c r="H25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="70" t="s">
-        <v>124</v>
+      <c r="B26" s="67" t="s">
+        <v>123</v>
       </c>
       <c r="C26" s="44" t="s">
         <v>12</v>
@@ -1971,25 +1977,25 @@
         <v>2.76E-2</v>
       </c>
       <c r="F26" s="45">
-        <f>E26*D26</f>
+        <f t="shared" si="1"/>
         <v>5.5199999999999999E-2</v>
       </c>
       <c r="G26" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="70" t="s">
-        <v>126</v>
+      <c r="B27" s="67" t="s">
+        <v>125</v>
       </c>
       <c r="C27" s="44" t="s">
         <v>12</v>
@@ -2002,25 +2008,25 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="F27" s="45">
-        <f>E27*D27</f>
+        <f t="shared" si="1"/>
         <v>0.17699999999999999</v>
       </c>
       <c r="G27" s="48" t="s">
         <v>40</v>
       </c>
       <c r="H27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="70" t="s">
-        <v>125</v>
+      <c r="B28" s="67" t="s">
+        <v>124</v>
       </c>
       <c r="C28" s="44" t="s">
         <v>12</v>
@@ -2033,25 +2039,25 @@
         <v>6.8999999999999992E-2</v>
       </c>
       <c r="F28" s="45">
-        <f>E28*D28</f>
+        <f t="shared" si="1"/>
         <v>6.8999999999999992E-2</v>
       </c>
       <c r="G28" s="27" t="s">
         <v>45</v>
       </c>
       <c r="H28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="70" t="s">
-        <v>127</v>
+      <c r="B29" s="67" t="s">
+        <v>126</v>
       </c>
       <c r="C29" s="44" t="s">
         <v>12</v>
@@ -2064,25 +2070,25 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="F29" s="45">
-        <f>E29*D29</f>
+        <f t="shared" si="1"/>
         <v>0.39600000000000002</v>
       </c>
       <c r="G29" s="27" t="s">
         <v>46</v>
       </c>
       <c r="H29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="70" t="s">
-        <v>128</v>
+      <c r="B30" s="67" t="s">
+        <v>127</v>
       </c>
       <c r="C30" s="44" t="s">
         <v>12</v>
@@ -2095,25 +2101,25 @@
         <v>0.13799999999999998</v>
       </c>
       <c r="F30" s="45">
-        <f>E30*D30</f>
+        <f t="shared" si="1"/>
         <v>0.13799999999999998</v>
       </c>
       <c r="G30" s="27" t="s">
         <v>47</v>
       </c>
       <c r="H30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="70" t="s">
-        <v>129</v>
+      <c r="B31" s="67" t="s">
+        <v>128</v>
       </c>
       <c r="C31" s="44" t="s">
         <v>12</v>
@@ -2126,25 +2132,25 @@
         <v>0.24900000000000003</v>
       </c>
       <c r="F31" s="45">
-        <f>E31*D31</f>
+        <f t="shared" si="1"/>
         <v>0.24900000000000003</v>
       </c>
       <c r="G31" s="27" t="s">
         <v>49</v>
       </c>
       <c r="H31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="70" t="s">
-        <v>130</v>
+      <c r="B32" s="67" t="s">
+        <v>129</v>
       </c>
       <c r="C32" s="44" t="s">
         <v>12</v>
@@ -2157,25 +2163,25 @@
         <v>0.24900000000000003</v>
       </c>
       <c r="F32" s="45">
-        <f>E32*D32</f>
+        <f t="shared" si="1"/>
         <v>0.24900000000000003</v>
       </c>
       <c r="G32" s="27" t="s">
         <v>50</v>
       </c>
       <c r="H32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="70" t="s">
-        <v>131</v>
+      <c r="B33" s="67" t="s">
+        <v>130</v>
       </c>
       <c r="C33" s="44" t="s">
         <v>12</v>
@@ -2188,25 +2194,25 @@
         <v>0.24900000000000003</v>
       </c>
       <c r="F33" s="45">
-        <f>E33*D33</f>
+        <f t="shared" si="1"/>
         <v>0.24900000000000003</v>
       </c>
       <c r="G33" s="27" t="s">
         <v>51</v>
       </c>
       <c r="H33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="70" t="s">
-        <v>132</v>
+      <c r="B34" s="67" t="s">
+        <v>131</v>
       </c>
       <c r="C34" s="44" t="s">
         <v>12</v>
@@ -2219,25 +2225,25 @@
         <v>0.24900000000000003</v>
       </c>
       <c r="F34" s="45">
-        <f>E34*D34</f>
+        <f t="shared" si="1"/>
         <v>0.24900000000000003</v>
       </c>
       <c r="G34" s="27" t="s">
         <v>52</v>
       </c>
       <c r="H34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="70" t="s">
-        <v>133</v>
+      <c r="B35" s="67" t="s">
+        <v>132</v>
       </c>
       <c r="C35" s="44" t="s">
         <v>12</v>
@@ -2250,25 +2256,25 @@
         <v>0.23500000000000001</v>
       </c>
       <c r="F35" s="45">
-        <f>E35*D35</f>
+        <f t="shared" si="1"/>
         <v>1.8800000000000001</v>
       </c>
       <c r="G35" s="27" t="s">
         <v>53</v>
       </c>
       <c r="H35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="70" t="s">
-        <v>134</v>
+      <c r="B36" s="67" t="s">
+        <v>133</v>
       </c>
       <c r="C36" s="44" t="s">
         <v>12</v>
@@ -2281,25 +2287,25 @@
         <v>0.23500000000000001</v>
       </c>
       <c r="F36" s="45">
-        <f>E36*D36</f>
+        <f t="shared" si="1"/>
         <v>1.8800000000000001</v>
       </c>
       <c r="G36" s="27" t="s">
         <v>54</v>
       </c>
       <c r="H36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="70" t="s">
-        <v>135</v>
+      <c r="B37" s="67" t="s">
+        <v>134</v>
       </c>
       <c r="C37" s="44" t="s">
         <v>12</v>
@@ -2312,25 +2318,25 @@
         <v>0.215</v>
       </c>
       <c r="F37" s="45">
-        <f>E37*D37</f>
+        <f t="shared" si="1"/>
         <v>0.64500000000000002</v>
       </c>
       <c r="G37" s="27" t="s">
         <v>62</v>
       </c>
       <c r="H37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="70" t="s">
-        <v>136</v>
+      <c r="B38" s="67" t="s">
+        <v>135</v>
       </c>
       <c r="C38" s="44" t="s">
         <v>12</v>
@@ -2339,29 +2345,29 @@
         <v>2</v>
       </c>
       <c r="E38" s="45">
-        <f t="shared" ref="E38:E40" si="0">2.15/10</f>
+        <f t="shared" ref="E38:E40" si="2">2.15/10</f>
         <v>0.215</v>
       </c>
       <c r="F38" s="45">
-        <f>E38*D38</f>
+        <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
       <c r="G38" s="27" t="s">
         <v>63</v>
       </c>
       <c r="H38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="70" t="s">
-        <v>137</v>
+      <c r="B39" s="67" t="s">
+        <v>136</v>
       </c>
       <c r="C39" s="44" t="s">
         <v>12</v>
@@ -2370,29 +2376,29 @@
         <v>2</v>
       </c>
       <c r="E39" s="45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.215</v>
       </c>
       <c r="F39" s="45">
-        <f>E39*D39</f>
+        <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
       <c r="G39" s="27" t="s">
         <v>68</v>
       </c>
       <c r="H39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="70" t="s">
-        <v>138</v>
+      <c r="B40" s="67" t="s">
+        <v>137</v>
       </c>
       <c r="C40" s="44" t="s">
         <v>12</v>
@@ -2401,29 +2407,29 @@
         <v>2</v>
       </c>
       <c r="E40" s="45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.215</v>
       </c>
       <c r="F40" s="45">
-        <f>E40*D40</f>
+        <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
       <c r="G40" s="27" t="s">
         <v>67</v>
       </c>
       <c r="H40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" s="70" t="s">
-        <v>139</v>
+        <v>106</v>
+      </c>
+      <c r="B41" s="67" t="s">
+        <v>138</v>
       </c>
       <c r="C41" s="44" t="s">
         <v>12</v>
@@ -2436,25 +2442,25 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="F41" s="45">
-        <f>E41*D41</f>
+        <f t="shared" si="1"/>
         <v>0.66500000000000004</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B42" s="70" t="s">
-        <v>140</v>
+        <v>105</v>
+      </c>
+      <c r="B42" s="67" t="s">
+        <v>139</v>
       </c>
       <c r="C42" s="44" t="s">
         <v>12</v>
@@ -2467,25 +2473,25 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="F42" s="45">
-        <f>E42*D42</f>
+        <f t="shared" si="1"/>
         <v>0.53200000000000003</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="67" t="s">
-        <v>141</v>
+      <c r="B43" s="64" t="s">
+        <v>140</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>9</v>
@@ -2498,24 +2504,24 @@
         <v>0.8</v>
       </c>
       <c r="F43" s="39">
-        <f>E43*D43</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="G43" s="21" t="s">
         <v>70</v>
       </c>
       <c r="H43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="68"/>
+      <c r="B44" s="65"/>
       <c r="C44" s="40" t="s">
         <v>14</v>
       </c>
@@ -2523,11 +2529,12 @@
         <v>1</v>
       </c>
       <c r="E44" s="41">
-        <v>19</v>
+        <f>19/40</f>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F44" s="41">
-        <f>E44*D44</f>
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>0.47499999999999998</v>
       </c>
       <c r="G44" s="23" t="s">
         <v>70</v>
@@ -2541,9 +2548,9 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="68"/>
+        <v>147</v>
+      </c>
+      <c r="B45" s="65"/>
       <c r="C45" s="40" t="s">
         <v>14</v>
       </c>
@@ -2551,14 +2558,15 @@
         <v>1</v>
       </c>
       <c r="E45" s="41">
-        <v>5</v>
+        <f>5/40</f>
+        <v>0.125</v>
       </c>
       <c r="F45" s="41">
-        <f>E45*D45</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>0.125</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>28</v>
@@ -2569,9 +2577,9 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="68"/>
+        <v>73</v>
+      </c>
+      <c r="B46" s="65"/>
       <c r="C46" s="40" t="s">
         <v>14</v>
       </c>
@@ -2579,14 +2587,15 @@
         <v>1</v>
       </c>
       <c r="E46" s="41">
-        <v>8.99</v>
+        <f>8.99/40</f>
+        <v>0.22475000000000001</v>
       </c>
       <c r="F46" s="41">
-        <f>E46*D46</f>
-        <v>8.99</v>
+        <f t="shared" si="1"/>
+        <v>0.22475000000000001</v>
       </c>
       <c r="G46" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>28</v>
@@ -2596,147 +2605,176 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="69" t="s">
-        <v>142</v>
-      </c>
-      <c r="C47" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="42">
-        <v>12</v>
-      </c>
-      <c r="E47" s="43">
-        <f>7.2/100</f>
-        <v>7.2000000000000008E-2</v>
-      </c>
-      <c r="F47" s="43">
-        <f>E47*D47</f>
-        <v>0.8640000000000001</v>
-      </c>
-      <c r="G47" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H47" t="s">
-        <v>89</v>
-      </c>
-      <c r="I47" t="s">
-        <v>90</v>
+      <c r="A47" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="65"/>
+      <c r="C47" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="40">
+        <v>1</v>
+      </c>
+      <c r="E47" s="41">
+        <v>0</v>
+      </c>
+      <c r="F47" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="69" t="s">
-        <v>143</v>
+      <c r="B48" s="66" t="s">
+        <v>141</v>
       </c>
       <c r="C48" s="42" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="42">
+        <v>12</v>
+      </c>
+      <c r="E48" s="43">
+        <f>7.2/100</f>
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="F48" s="43">
+        <f t="shared" si="1"/>
+        <v>0.8640000000000001</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H48" t="s">
+        <v>88</v>
+      </c>
+      <c r="I48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="42">
         <v>4</v>
       </c>
-      <c r="E48" s="43">
+      <c r="E49" s="43">
         <f>7/100</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F48" s="43">
-        <f>E48*D48</f>
+      <c r="F49" s="43">
+        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="G48" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H48" t="s">
-        <v>89</v>
-      </c>
-      <c r="I48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="20" t="s">
+      <c r="G49" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" t="s">
+        <v>88</v>
+      </c>
+      <c r="I49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="38">
+        <v>1</v>
+      </c>
+      <c r="E50" s="39">
+        <v>3.82</v>
+      </c>
+      <c r="F50" s="39">
+        <f t="shared" si="1"/>
+        <v>3.82</v>
+      </c>
+      <c r="G50" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="C49" s="38" t="s">
+      <c r="H50" t="s">
+        <v>88</v>
+      </c>
+      <c r="I50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="68"/>
+      <c r="C51" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="38">
-        <v>1</v>
-      </c>
-      <c r="E49" s="39">
-        <v>3.82</v>
-      </c>
-      <c r="F49" s="39">
-        <f>E49*D49</f>
-        <v>3.82</v>
-      </c>
-      <c r="G49" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H49" t="s">
-        <v>89</v>
-      </c>
-      <c r="I49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="71"/>
-      <c r="C50" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="46">
+      <c r="D51" s="46">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E50" s="47">
+      <c r="E51" s="47">
         <f>5.16/4</f>
         <v>1.29</v>
       </c>
-      <c r="F50" s="47">
-        <f>E50*D50</f>
+      <c r="F51" s="47">
+        <f t="shared" si="1"/>
         <v>1.29</v>
       </c>
-      <c r="G50" s="31"/>
-      <c r="H50" s="2" t="s">
+      <c r="G51" s="31"/>
+      <c r="H51" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="49"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="1">
-        <f>SUM(F10:F50)</f>
-        <v>389.78528062605761</v>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="69"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="1">
+        <f>SUM(F10:F51)</f>
+        <v>357.6200306260576</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:E52"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G45" r:id="rId1" location="shipping-estimate" xr:uid="{936C8A8D-5899-404F-8CD0-80610CA9332C}"/>
-    <hyperlink ref="G47" r:id="rId2" display="https://www.amazon.com/Adiyer-Stainless-Phillips-Countersunk-Tapping/dp/B07VSVM9ZP/ref=sr_1_1_sspa?keywords=m2+10mm+wood+screws&amp;qid=1576017761&amp;s=hi&amp;sr=1-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyR1lDRU1BTE5XTlo0JmVuY3J5cHRlZElkPUEwNjI3MzQ4MUtES1VLSkhVWElNOSZlbmNyeXB0ZWRBZElkPUEwOTc5OTA3MVdSMVA1TUNQU1oxQyZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{8BA7C019-7D73-174A-9F60-6C56DA48A3C7}"/>
+    <hyperlink ref="G48" r:id="rId2" display="https://www.amazon.com/Adiyer-Stainless-Phillips-Countersunk-Tapping/dp/B07VSVM9ZP/ref=sr_1_1_sspa?keywords=m2+10mm+wood+screws&amp;qid=1576017761&amp;s=hi&amp;sr=1-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyR1lDRU1BTE5XTlo0JmVuY3J5cHRlZElkPUEwNjI3MzQ4MUtES1VLSkhVWElNOSZlbmNyeXB0ZWRBZElkPUEwOTc5OTA3MVdSMVA1TUNQU1oxQyZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{8BA7C019-7D73-174A-9F60-6C56DA48A3C7}"/>
     <hyperlink ref="G27" r:id="rId3" xr:uid="{9898932F-206F-8047-A040-01385F905E2B}"/>
+    <hyperlink ref="G47" r:id="rId4" xr:uid="{8C816692-8A58-874A-9DBB-D5F28B275639}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>